<commit_message>
chapter e id no planejamento e funcionalidade buscar profissional no product
</commit_message>
<xml_diff>
--- a/documentos/analise-de-projeto/planejamento-sprint-1.xlsx
+++ b/documentos/analise-de-projeto/planejamento-sprint-1.xlsx
@@ -78,9 +78,6 @@
     <t>Script BD</t>
   </si>
   <si>
-    <t>Criar Repositório</t>
-  </si>
-  <si>
     <t>Esforço</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>Apresentar aos colegas</t>
   </si>
   <si>
-    <t>Criar Ambiente de Desenvolvimento</t>
-  </si>
-  <si>
     <t>Instalar Netbeans 8.0</t>
   </si>
   <si>
@@ -174,13 +168,19 @@
     <t>Criar classe</t>
   </si>
   <si>
-    <t>Estória de Usuário: CH:4 ID:4 , CH:2 ID:3 - Contato cliente/profissional</t>
-  </si>
-  <si>
-    <t>()</t>
-  </si>
-  <si>
     <t>não tem dependencia</t>
+  </si>
+  <si>
+    <t>Estória de Usuário: CH:2, CH:4 ID:10 - Contato cliente/profissional</t>
+  </si>
+  <si>
+    <t>Estória de Usuário: CH:5 ID:24 - Criar Repositório GITHUB</t>
+  </si>
+  <si>
+    <t>Estória de Usuário: CH:5 ID:25 - Criar Ambiente de Desenvolvimento</t>
+  </si>
+  <si>
+    <t>Todos</t>
   </si>
 </sst>
 </file>
@@ -254,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -276,6 +276,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -682,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -712,14 +713,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="A6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -817,7 +818,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -836,14 +837,14 @@
       <c r="E15" s="7"/>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="A17" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -853,13 +854,13 @@
         <v>4</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>7</v>
@@ -867,13 +868,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="7">
         <v>42450</v>
@@ -882,18 +883,18 @@
         <v>42450</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" s="7">
         <v>42450</v>
@@ -902,18 +903,18 @@
         <v>42450</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="7">
         <v>42450</v>
@@ -922,18 +923,18 @@
         <v>42450</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22" s="7">
         <v>42450</v>
@@ -942,18 +943,18 @@
         <v>42450</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="7">
         <v>42450</v>
@@ -962,18 +963,18 @@
         <v>42450</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D24" s="7">
         <v>42450</v>
@@ -982,18 +983,18 @@
         <v>42450</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" s="7">
         <v>42453</v>
@@ -1002,34 +1003,34 @@
         <v>42453</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="1:7" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="1:7" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" spans="1:7" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -1039,10 +1040,10 @@
         <v>4</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>6</v>
@@ -1053,13 +1054,13 @@
     </row>
     <row r="30" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="12">
         <v>42453</v>
@@ -1067,16 +1068,17 @@
       <c r="E30" s="12">
         <v>42453</v>
       </c>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="12">
         <v>42453</v>
@@ -1087,13 +1089,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="9">
         <v>42453</v>
@@ -1104,13 +1106,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" s="9">
         <v>42453</v>
@@ -1121,13 +1123,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D34" s="9">
         <v>42453</v>
@@ -1138,7 +1140,7 @@
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -1154,10 +1156,10 @@
         <v>4</v>
       </c>
       <c r="C37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>6</v>
@@ -1168,10 +1170,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1181,17 +1183,17 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1203,7 +1205,7 @@
     <mergeCell ref="A28:F28"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.13888888888888901" bottom="0.13888888888888901" header="0" footer="0"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;10Página &amp;P</oddFooter>

</xml_diff>

<commit_message>
posto chapter e id na tarefa CRUD
</commit_message>
<xml_diff>
--- a/documentos/analise-de-projeto/planejamento-sprint-1.xlsx
+++ b/documentos/analise-de-projeto/planejamento-sprint-1.xlsx
@@ -249,10 +249,10 @@
     <t>06/03/2-16</t>
   </si>
   <si>
-    <t>Estória de  Usuário: Realizar CRUD cliente e profissional</t>
-  </si>
-  <si>
     <t>Estória de  Usuário: CH:6 ID:27 - Estudar API de mapas</t>
+  </si>
+  <si>
+    <t>Estória de  Usuário: CH:1 ID:1 e 2- Cadastrar Cliente e Profissional - CRUD</t>
   </si>
 </sst>
 </file>
@@ -362,6 +362,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -369,10 +373,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -805,14 +805,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -998,14 +998,14 @@
       <c r="E15" s="6"/>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -1195,30 +1195,30 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
     </row>
     <row r="28" spans="1:8" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
     </row>
     <row r="29" spans="1:8" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -1444,10 +1444,10 @@
       <c r="D40" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E40" s="23">
+      <c r="E40" s="20">
         <v>42464</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="20">
         <v>42464</v>
       </c>
     </row>
@@ -1464,10 +1464,10 @@
       <c r="D41" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="23">
+      <c r="E41" s="20">
         <v>42464</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F41" s="20">
         <v>42464</v>
       </c>
     </row>
@@ -1484,10 +1484,10 @@
       <c r="D42" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E42" s="23">
+      <c r="E42" s="20">
         <v>42465</v>
       </c>
-      <c r="F42" s="23">
+      <c r="F42" s="20">
         <v>42465</v>
       </c>
       <c r="G42" s="10"/>
@@ -1505,10 +1505,10 @@
       <c r="D43" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E43" s="23">
+      <c r="E43" s="20">
         <v>42465</v>
       </c>
-      <c r="F43" s="23">
+      <c r="F43" s="20">
         <v>42465</v>
       </c>
     </row>
@@ -1525,10 +1525,10 @@
       <c r="D44" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E44" s="23">
+      <c r="E44" s="20">
         <v>42465</v>
       </c>
-      <c r="F44" s="23">
+      <c r="F44" s="20">
         <v>42465</v>
       </c>
     </row>
@@ -1545,10 +1545,10 @@
       <c r="D45" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="23">
+      <c r="E45" s="20">
         <v>42466</v>
       </c>
-      <c r="F45" s="23">
+      <c r="F45" s="20">
         <v>42466</v>
       </c>
       <c r="G45" s="10"/>
@@ -1566,10 +1566,10 @@
       <c r="D46" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E46" s="23">
+      <c r="E46" s="20">
         <v>42466</v>
       </c>
-      <c r="F46" s="23">
+      <c r="F46" s="20">
         <v>42466</v>
       </c>
     </row>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="C48" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
@@ -1687,10 +1687,10 @@
     </row>
     <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="C54" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D54" s="14"/>
-      <c r="E54" s="22"/>
+      <c r="E54" s="19"/>
       <c r="F54" s="14"/>
       <c r="G54" s="9"/>
     </row>

</xml_diff>